<commit_message>
Add Procfile and update config/requirements for email and deployment
</commit_message>
<xml_diff>
--- a/data/mahasiswa.xlsx
+++ b/data/mahasiswa.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="46">
   <si>
     <t>nama</t>
   </si>
@@ -37,31 +37,112 @@
     <t>Azka Insan Robbani</t>
   </si>
   <si>
-    <t>jason cornelius cha</t>
-  </si>
-  <si>
-    <t>eko</t>
-  </si>
-  <si>
-    <t>davrielle</t>
+    <t>Jason Cornelius Cha</t>
+  </si>
+  <si>
+    <t>Eko Prasetyo</t>
+  </si>
+  <si>
+    <t>Davrielle Saddad</t>
+  </si>
+  <si>
+    <t>Fathur Rachman</t>
+  </si>
+  <si>
+    <t>Vina Aulia</t>
+  </si>
+  <si>
+    <t>Satria Apriza Fajar</t>
+  </si>
+  <si>
+    <t>Dea Amellya</t>
+  </si>
+  <si>
+    <t>Ahmad Firdaus</t>
+  </si>
+  <si>
+    <t>Ade Sofyan</t>
+  </si>
+  <si>
+    <t>Dimas Ahmad</t>
+  </si>
+  <si>
+    <t>Maulana Ikhsan Fadhillah</t>
+  </si>
+  <si>
+    <t>Bagus Ardiansyah</t>
+  </si>
+  <si>
+    <t>Tumpal Sinaga</t>
+  </si>
+  <si>
+    <t>Jandri Hartat Gea</t>
+  </si>
+  <si>
+    <t>Walman Pangaribuan</t>
+  </si>
+  <si>
+    <t>Rafli Pratama</t>
+  </si>
+  <si>
+    <t>Nazril Supriyadi</t>
+  </si>
+  <si>
+    <t>Muhammad Alif Fajriansyah</t>
+  </si>
+  <si>
+    <t>Dzaki Ramadhan</t>
+  </si>
+  <si>
+    <t>Servatius Hasta Kristanto</t>
+  </si>
+  <si>
+    <t>Ade Jahwa Aulia</t>
+  </si>
+  <si>
+    <t>Azmi Al Fahriza</t>
+  </si>
+  <si>
+    <t>Gregorius Gilbert Ieli Sarjana</t>
+  </si>
+  <si>
+    <t>12dwq21</t>
+  </si>
+  <si>
+    <t>hm</t>
   </si>
   <si>
     <t>Laki-laki</t>
   </si>
   <si>
+    <t>Perempuan</t>
+  </si>
+  <si>
     <t>03TPLP002</t>
   </si>
   <si>
     <t>03TPLP009</t>
   </si>
   <si>
-    <t>Manajemen</t>
-  </si>
-  <si>
-    <t>DKV</t>
+    <t>123d32r4</t>
+  </si>
+  <si>
+    <t>20TPLPM0020</t>
+  </si>
+  <si>
+    <t>Sistem Informasi</t>
+  </si>
+  <si>
+    <t>Desain Komunikas Visual</t>
   </si>
   <si>
     <t>Teknik Informatika</t>
+  </si>
+  <si>
+    <t>Matematika</t>
+  </si>
+  <si>
+    <t>Biologi</t>
   </si>
   <si>
     <t>Non Aktif</t>
@@ -428,7 +509,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -462,16 +543,16 @@
         <v>241011400099</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -482,16 +563,16 @@
         <v>241011402427</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="F3" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -502,16 +583,16 @@
         <v>241011400022</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="F4" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -522,16 +603,456 @@
         <v>241011400065</v>
       </c>
       <c r="C5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="D5" t="s">
+      <c r="B6">
+        <v>241011401713</v>
+      </c>
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
         <v>11</v>
       </c>
-      <c r="E5" t="s">
+      <c r="B7">
+        <v>241011401650</v>
+      </c>
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8">
+        <v>241011400103</v>
+      </c>
+      <c r="C8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9">
+        <v>241011400089</v>
+      </c>
+      <c r="C9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10">
+        <v>241011401761</v>
+      </c>
+      <c r="C10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
         <v>15</v>
       </c>
-      <c r="F5" t="s">
+      <c r="B11">
+        <v>241011402338</v>
+      </c>
+      <c r="C11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12">
+        <v>241011402835</v>
+      </c>
+      <c r="C12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
         <v>17</v>
+      </c>
+      <c r="B13">
+        <v>241011400092</v>
+      </c>
+      <c r="C13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14">
+        <v>241011401958</v>
+      </c>
+      <c r="C14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" t="s">
+        <v>40</v>
+      </c>
+      <c r="F14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15">
+        <v>241011400087</v>
+      </c>
+      <c r="C15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" t="s">
+        <v>40</v>
+      </c>
+      <c r="F15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16">
+        <v>241012402295</v>
+      </c>
+      <c r="C16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E16" t="s">
+        <v>40</v>
+      </c>
+      <c r="F16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17">
+        <v>241011400094</v>
+      </c>
+      <c r="C17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17" t="s">
+        <v>40</v>
+      </c>
+      <c r="F17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18">
+        <v>241011400075</v>
+      </c>
+      <c r="C18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" t="s">
+        <v>40</v>
+      </c>
+      <c r="F18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19">
+        <v>241011400091</v>
+      </c>
+      <c r="C19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E19" t="s">
+        <v>40</v>
+      </c>
+      <c r="F19" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20">
+        <v>241011402197</v>
+      </c>
+      <c r="C20" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" t="s">
+        <v>34</v>
+      </c>
+      <c r="E20" t="s">
+        <v>40</v>
+      </c>
+      <c r="F20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21">
+        <v>241011400097</v>
+      </c>
+      <c r="C21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" t="s">
+        <v>34</v>
+      </c>
+      <c r="E21" t="s">
+        <v>40</v>
+      </c>
+      <c r="F21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22">
+        <v>241011400076</v>
+      </c>
+      <c r="C22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E22" t="s">
+        <v>40</v>
+      </c>
+      <c r="F22" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23">
+        <v>241011402829</v>
+      </c>
+      <c r="C23" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23" t="s">
+        <v>34</v>
+      </c>
+      <c r="E23" t="s">
+        <v>40</v>
+      </c>
+      <c r="F23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24">
+        <v>241011403269</v>
+      </c>
+      <c r="C24" t="s">
+        <v>32</v>
+      </c>
+      <c r="D24" t="s">
+        <v>34</v>
+      </c>
+      <c r="E24" t="s">
+        <v>40</v>
+      </c>
+      <c r="F24" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25">
+        <v>241011402382</v>
+      </c>
+      <c r="C25" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25" t="s">
+        <v>34</v>
+      </c>
+      <c r="E25" t="s">
+        <v>42</v>
+      </c>
+      <c r="F25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26">
+        <v>123456789101</v>
+      </c>
+      <c r="C26" t="s">
+        <v>32</v>
+      </c>
+      <c r="D26" t="s">
+        <v>36</v>
+      </c>
+      <c r="E26" t="s">
+        <v>40</v>
+      </c>
+      <c r="F26" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27">
+        <v>123456789109</v>
+      </c>
+      <c r="C27" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27" t="s">
+        <v>37</v>
+      </c>
+      <c r="E27" t="s">
+        <v>42</v>
+      </c>
+      <c r="F27" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>